<commit_message>
New version of exp definitions
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen_bsort_xrtos_pi3.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen_bsort_xrtos_pi3.xlsx
@@ -109,25 +109,25 @@
     <t xml:space="preserve">'1'</t>
   </si>
   <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'4679'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE4000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES1_INPUTSIZE6000</t>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'5689'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE6000</t>
   </si>
   <si>
     <t xml:space="preserve">'2111'</t>
@@ -136,22 +136,22 @@
     <t xml:space="preserve">'1222'</t>
   </si>
   <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE4000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_PI3_XRTOS_CORES4_WRITEATTACK1_INPUTSIZE6000</t>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE6000</t>
   </si>
 </sst>
 </file>
@@ -278,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,10 +340,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,10 +431,10 @@
   <dimension ref="A1:AMJ68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -958,7 +954,7 @@
         <f aca="false">A8+1</f>
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -970,19 +966,19 @@
       <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="17" t="n">
+      <c r="F9" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H9" s="17" t="n">
+      <c r="H9" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1009,7 +1005,7 @@
       <c r="Q9" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R9" s="18" t="n">
+      <c r="R9" s="17" t="n">
         <f aca="false">INT(T9/U9)</f>
         <v>654</v>
       </c>
@@ -1017,7 +1013,7 @@
         <f aca="false">S$3</f>
         <v>58929</v>
       </c>
-      <c r="T9" s="18" t="n">
+      <c r="T9" s="17" t="n">
         <f aca="false">INT(S9/10)</f>
         <v>5892</v>
       </c>
@@ -1030,7 +1026,7 @@
         <f aca="false">A9+1</f>
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -1042,19 +1038,19 @@
       <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="17" t="n">
+      <c r="F10" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H10" s="17" t="n">
+      <c r="H10" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -1081,7 +1077,7 @@
       <c r="Q10" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R10" s="18" t="n">
+      <c r="R10" s="17" t="n">
         <f aca="false">INT(T10/U10)</f>
         <v>14960</v>
       </c>
@@ -1089,7 +1085,7 @@
         <f aca="false">S$4</f>
         <v>1346436</v>
       </c>
-      <c r="T10" s="18" t="n">
+      <c r="T10" s="17" t="n">
         <f aca="false">INT(S10/10)</f>
         <v>134643</v>
       </c>
@@ -1102,7 +1098,7 @@
         <f aca="false">A10+1</f>
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -1114,19 +1110,19 @@
       <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="17" t="n">
+      <c r="F11" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H11" s="17" t="n">
+      <c r="H11" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1153,7 +1149,7 @@
       <c r="Q11" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R11" s="18" t="n">
+      <c r="R11" s="17" t="n">
         <f aca="false">INT(T11/U11)</f>
         <v>59510</v>
       </c>
@@ -1161,7 +1157,7 @@
         <f aca="false">S$5</f>
         <v>5355925</v>
       </c>
-      <c r="T11" s="18" t="n">
+      <c r="T11" s="17" t="n">
         <f aca="false">INT(S11/10)</f>
         <v>535592</v>
       </c>
@@ -1174,7 +1170,7 @@
         <f aca="false">A11+1</f>
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -1186,19 +1182,19 @@
       <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="17" t="n">
+      <c r="F12" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H12" s="17" t="n">
+      <c r="H12" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1225,7 +1221,7 @@
       <c r="Q12" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R12" s="18" t="n">
+      <c r="R12" s="17" t="n">
         <f aca="false">INT(T12/U12)</f>
         <v>236252</v>
       </c>
@@ -1233,7 +1229,7 @@
         <f aca="false">S$6</f>
         <v>21262688</v>
       </c>
-      <c r="T12" s="18" t="n">
+      <c r="T12" s="17" t="n">
         <f aca="false">INT(S12/10)</f>
         <v>2126268</v>
       </c>
@@ -1246,7 +1242,7 @@
         <f aca="false">A12+1</f>
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="0" t="n">
@@ -1258,19 +1254,19 @@
       <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="17" t="n">
+      <c r="F13" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H13" s="17" t="n">
+      <c r="H13" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1297,7 +1293,7 @@
       <c r="Q13" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R13" s="18" t="n">
+      <c r="R13" s="17" t="n">
         <f aca="false">INT(T13/U13)</f>
         <v>938850</v>
       </c>
@@ -1305,7 +1301,7 @@
         <f aca="false">S$7</f>
         <v>84496533</v>
       </c>
-      <c r="T13" s="18" t="n">
+      <c r="T13" s="17" t="n">
         <f aca="false">INT(S13/10)</f>
         <v>8449653</v>
       </c>
@@ -1318,7 +1314,7 @@
         <f aca="false">A13+1</f>
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -1330,19 +1326,19 @@
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="17" t="n">
+      <c r="F14" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="16" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H14" s="17" t="n">
+      <c r="H14" s="16" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1369,7 +1365,7 @@
       <c r="Q14" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R14" s="18" t="n">
+      <c r="R14" s="17" t="n">
         <f aca="false">INT(T14/U14)</f>
         <v>2108042</v>
       </c>
@@ -1377,7 +1373,7 @@
         <f aca="false">S$8</f>
         <v>189723795</v>
       </c>
-      <c r="T14" s="18" t="n">
+      <c r="T14" s="17" t="n">
         <f aca="false">INT(S14/10)</f>
         <v>18972379</v>
       </c>
@@ -1393,9 +1389,9 @@
       <c r="C15" s="0"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -1407,9 +1403,9 @@
       <c r="C16" s="0"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1421,9 +1417,9 @@
       <c r="C17" s="0"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1435,9 +1431,9 @@
       <c r="C18" s="0"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1449,9 +1445,9 @@
       <c r="C19" s="0"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1463,9 +1459,9 @@
       <c r="C20" s="0"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1477,9 +1473,9 @@
       <c r="C21" s="0"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1491,9 +1487,9 @@
       <c r="C22" s="0"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1505,9 +1501,9 @@
       <c r="C23" s="0"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1524,9 +1520,9 @@
       <c r="C24" s="0"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1543,9 +1539,9 @@
       <c r="C25" s="0"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1562,9 +1558,9 @@
       <c r="C26" s="0"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1581,9 +1577,9 @@
       <c r="C27" s="0"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1600,9 +1596,9 @@
       <c r="C28" s="0"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1619,9 +1615,9 @@
       <c r="C29" s="0"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1638,9 +1634,9 @@
       <c r="C30" s="0"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1657,9 +1653,9 @@
       <c r="C31" s="0"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1676,9 +1672,9 @@
       <c r="C32" s="0"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1695,9 +1691,9 @@
       <c r="C33" s="0"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1714,9 +1710,9 @@
       <c r="C34" s="0"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1733,9 +1729,9 @@
       <c r="C35" s="0"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1752,9 +1748,9 @@
       <c r="C36" s="0"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1771,9 +1767,9 @@
       <c r="C37" s="0"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1790,9 +1786,9 @@
       <c r="C38" s="0"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1809,9 +1805,9 @@
       <c r="C39" s="0"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1828,9 +1824,9 @@
       <c r="C40" s="0"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1847,9 +1843,9 @@
       <c r="C41" s="0"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -1866,9 +1862,9 @@
       <c r="C42" s="0"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -1885,9 +1881,9 @@
       <c r="C43" s="0"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -1904,9 +1900,9 @@
       <c r="C44" s="0"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -1923,9 +1919,9 @@
       <c r="C45" s="0"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -1942,9 +1938,9 @@
       <c r="C46" s="0"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -1961,9 +1957,9 @@
       <c r="C47" s="0"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -1980,9 +1976,9 @@
       <c r="C48" s="0"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -1999,9 +1995,9 @@
       <c r="C49" s="0"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2018,9 +2014,9 @@
       <c r="C50" s="0"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2037,9 +2033,9 @@
       <c r="C51" s="0"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2056,9 +2052,9 @@
       <c r="C52" s="0"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2075,9 +2071,9 @@
       <c r="C53" s="0"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2101,9 +2097,9 @@
       <c r="C55" s="0"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -2120,9 +2116,9 @@
       <c r="C56" s="0"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2139,9 +2135,9 @@
       <c r="C57" s="0"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2158,9 +2154,9 @@
       <c r="C58" s="0"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2177,9 +2173,9 @@
       <c r="C59" s="0"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2196,9 +2192,9 @@
       <c r="C60" s="0"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2215,9 +2211,9 @@
       <c r="C61" s="0"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2234,9 +2230,9 @@
       <c r="C62" s="0"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2253,9 +2249,9 @@
       <c r="C63" s="0"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2272,9 +2268,9 @@
       <c r="C64" s="0"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2291,9 +2287,9 @@
       <c r="C65" s="0"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2310,9 +2306,9 @@
       <c r="C66" s="0"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2329,9 +2325,9 @@
       <c r="C67" s="0"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2348,9 +2344,9 @@
       <c r="C68" s="0"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>

</xml_diff>

<commit_message>
Excel sheets with synbench_repeat param
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen_bsort_xrtos_pi3.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen_bsort_xrtos_pi3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t xml:space="preserve">xrtos or circle</t>
   </si>
@@ -100,6 +100,9 @@
     <t xml:space="preserve">cycles per count</t>
   </si>
   <si>
+    <t xml:space="preserve">synbench repeat</t>
+  </si>
+  <si>
     <t xml:space="preserve">xrtos</t>
   </si>
   <si>
@@ -130,6 +133,9 @@
     <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE6000</t>
   </si>
   <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE8000</t>
+  </si>
+  <si>
     <t xml:space="preserve">'2111'</t>
   </si>
   <si>
@@ -152,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES4_WRITEATTACK1_INPUTSIZE8000</t>
   </si>
 </sst>
 </file>
@@ -278,7 +287,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,8 +328,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -339,6 +348,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,6 +366,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -428,13 +449,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ68"/>
+  <dimension ref="A1:AMJ69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V16" activeCellId="0" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -556,7 +577,9 @@
       <c r="U2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="10"/>
+      <c r="V2" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="X2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
@@ -565,16 +588,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -589,10 +612,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
@@ -623,6 +646,7 @@
       <c r="U3" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="V3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
@@ -630,16 +654,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -654,10 +678,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -688,6 +712,7 @@
       <c r="U4" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="V4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="n">
@@ -695,16 +720,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -719,10 +744,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
@@ -753,6 +778,7 @@
       <c r="U5" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="V5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="n">
@@ -760,16 +786,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -784,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
@@ -818,6 +844,7 @@
       <c r="U6" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="V6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="n">
@@ -825,16 +852,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -849,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
@@ -883,6 +910,7 @@
       <c r="U7" s="11" t="n">
         <v>9</v>
       </c>
+      <c r="V7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
@@ -890,16 +918,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F8" s="12" t="n">
         <f aca="false">TRUE()</f>
@@ -914,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
@@ -948,468 +976,599 @@
       <c r="U8" s="11" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="n">
+      <c r="V8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="n">
         <f aca="false">A8+1</f>
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="12" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G9" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H9" s="16" t="n">
+      <c r="J9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11" t="n">
+        <v>8000</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="13" t="n">
+        <f aca="false">INT(T9/U9)</f>
+        <v>3743686</v>
+      </c>
+      <c r="S9" s="16" t="n">
+        <v>336931745</v>
+      </c>
+      <c r="T9" s="13" t="n">
+        <f aca="false">INT(S9/10)</f>
+        <v>33693174</v>
+      </c>
+      <c r="U9" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="V9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="n">
+        <f aca="false">A8+1</f>
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="1" t="n">
+      <c r="I10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O10" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P10" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q10" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R9" s="17" t="n">
-        <f aca="false">INT(T9/U9)</f>
+      <c r="R10" s="19" t="n">
+        <f aca="false">INT(T10/U10)</f>
         <v>654</v>
       </c>
-      <c r="S9" s="0" t="n">
+      <c r="S10" s="0" t="n">
         <f aca="false">S$3</f>
         <v>58929</v>
       </c>
-      <c r="T9" s="17" t="n">
-        <f aca="false">INT(S9/10)</f>
+      <c r="T10" s="19" t="n">
+        <f aca="false">INT(S10/10)</f>
         <v>5892</v>
       </c>
-      <c r="U9" s="0" t="n">
+      <c r="U10" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="n">
-        <f aca="false">A9+1</f>
+      <c r="V10" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
+        <f aca="false">A10+1</f>
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G10" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="16" t="n">
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="1" t="n">
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O11" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="P11" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="Q11" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R10" s="17" t="n">
-        <f aca="false">INT(T10/U10)</f>
+      <c r="R11" s="19" t="n">
+        <f aca="false">INT(T11/U11)</f>
         <v>14960</v>
       </c>
-      <c r="S10" s="0" t="n">
+      <c r="S11" s="0" t="n">
         <f aca="false">S$4</f>
         <v>1346436</v>
       </c>
-      <c r="T10" s="17" t="n">
-        <f aca="false">INT(S10/10)</f>
+      <c r="T11" s="19" t="n">
+        <f aca="false">INT(S11/10)</f>
         <v>134643</v>
       </c>
-      <c r="U10" s="0" t="n">
+      <c r="U11" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="n">
-        <f aca="false">A10+1</f>
+      <c r="V11" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="17" t="n">
+        <f aca="false">A11+1</f>
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="16" t="n">
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="1" t="n">
+      <c r="I12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O12" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P12" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q12" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R11" s="17" t="n">
-        <f aca="false">INT(T11/U11)</f>
+      <c r="R12" s="19" t="n">
+        <f aca="false">INT(T12/U12)</f>
         <v>59510</v>
       </c>
-      <c r="S11" s="0" t="n">
+      <c r="S12" s="0" t="n">
         <f aca="false">S$5</f>
         <v>5355925</v>
       </c>
-      <c r="T11" s="17" t="n">
-        <f aca="false">INT(S11/10)</f>
+      <c r="T12" s="19" t="n">
+        <f aca="false">INT(S12/10)</f>
         <v>535592</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="U12" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
-        <f aca="false">A11+1</f>
+      <c r="V12" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="n">
+        <f aca="false">A12+1</f>
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="16" t="n">
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="1" t="n">
+      <c r="I13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="1" t="n">
         <v>2000</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O13" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P13" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q13" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R12" s="17" t="n">
-        <f aca="false">INT(T12/U12)</f>
+      <c r="R13" s="19" t="n">
+        <f aca="false">INT(T13/U13)</f>
         <v>236252</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S13" s="0" t="n">
         <f aca="false">S$6</f>
         <v>21262688</v>
       </c>
-      <c r="T12" s="17" t="n">
-        <f aca="false">INT(S12/10)</f>
+      <c r="T13" s="19" t="n">
+        <f aca="false">INT(S13/10)</f>
         <v>2126268</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U13" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
-        <f aca="false">A12+1</f>
+      <c r="V13" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="n">
+        <f aca="false">A13+1</f>
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="16" t="n">
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="1" t="n">
+      <c r="I14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="1" t="n">
         <v>4000</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O14" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="P14" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q14" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R13" s="17" t="n">
-        <f aca="false">INT(T13/U13)</f>
+      <c r="R14" s="19" t="n">
+        <f aca="false">INT(T14/U14)</f>
         <v>938850</v>
       </c>
-      <c r="S13" s="0" t="n">
+      <c r="S14" s="0" t="n">
         <f aca="false">S$7</f>
         <v>84496533</v>
       </c>
-      <c r="T13" s="17" t="n">
-        <f aca="false">INT(S13/10)</f>
+      <c r="T14" s="19" t="n">
+        <f aca="false">INT(S14/10)</f>
         <v>8449653</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="U14" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="n">
-        <f aca="false">A13+1</f>
+      <c r="V14" s="20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
+        <f aca="false">A14+1</f>
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="16" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H14" s="16" t="n">
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="18" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="1" t="n">
+      <c r="I15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="1" t="n">
         <v>6000</v>
       </c>
-      <c r="O14" s="0" t="n">
+      <c r="O15" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="P14" s="0" t="n">
+      <c r="P15" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="Q14" s="0" t="n">
+      <c r="Q15" s="0" t="n">
         <v>1048576</v>
       </c>
-      <c r="R14" s="17" t="n">
-        <f aca="false">INT(T14/U14)</f>
+      <c r="R15" s="19" t="n">
+        <f aca="false">INT(T15/U15)</f>
         <v>2108042</v>
       </c>
-      <c r="S14" s="0" t="n">
+      <c r="S15" s="0" t="n">
         <f aca="false">S$8</f>
         <v>189723795</v>
       </c>
-      <c r="T14" s="17" t="n">
-        <f aca="false">INT(S14/10)</f>
+      <c r="T15" s="19" t="n">
+        <f aca="false">INT(S15/10)</f>
         <v>18972379</v>
       </c>
-      <c r="U14" s="0" t="n">
+      <c r="U15" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="V14" s="0"/>
-      <c r="W14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="V15" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="W15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="n">
+        <f aca="false">A15+1</f>
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="18" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="18" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="R16" s="19" t="n">
+        <f aca="false">INT(T16/U16)</f>
+        <v>3743686</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <f aca="false">S$9</f>
+        <v>336931745</v>
+      </c>
+      <c r="T16" s="19" t="n">
+        <f aca="false">INT(S16/10)</f>
+        <v>33693174</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="V16" s="20" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
@@ -1417,9 +1576,9 @@
       <c r="C17" s="0"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1431,9 +1590,9 @@
       <c r="C18" s="0"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1445,9 +1604,9 @@
       <c r="C19" s="0"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1459,9 +1618,9 @@
       <c r="C20" s="0"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1473,9 +1632,9 @@
       <c r="C21" s="0"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1487,9 +1646,9 @@
       <c r="C22" s="0"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1501,18 +1660,13 @@
       <c r="C23" s="0"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
@@ -1520,9 +1674,9 @@
       <c r="C24" s="0"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1539,9 +1693,9 @@
       <c r="C25" s="0"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1558,9 +1712,9 @@
       <c r="C26" s="0"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1577,9 +1731,9 @@
       <c r="C27" s="0"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1596,9 +1750,9 @@
       <c r="C28" s="0"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1615,9 +1769,9 @@
       <c r="C29" s="0"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1634,9 +1788,9 @@
       <c r="C30" s="0"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1653,9 +1807,9 @@
       <c r="C31" s="0"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1672,9 +1826,9 @@
       <c r="C32" s="0"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1691,9 +1845,9 @@
       <c r="C33" s="0"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1710,9 +1864,9 @@
       <c r="C34" s="0"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1729,9 +1883,9 @@
       <c r="C35" s="0"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1748,9 +1902,9 @@
       <c r="C36" s="0"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1767,9 +1921,9 @@
       <c r="C37" s="0"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1786,9 +1940,9 @@
       <c r="C38" s="0"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1805,9 +1959,9 @@
       <c r="C39" s="0"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1824,9 +1978,9 @@
       <c r="C40" s="0"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1843,9 +1997,9 @@
       <c r="C41" s="0"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -1862,9 +2016,9 @@
       <c r="C42" s="0"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -1881,9 +2035,9 @@
       <c r="C43" s="0"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -1900,9 +2054,9 @@
       <c r="C44" s="0"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -1919,9 +2073,9 @@
       <c r="C45" s="0"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -1938,9 +2092,9 @@
       <c r="C46" s="0"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -1957,9 +2111,9 @@
       <c r="C47" s="0"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -1976,9 +2130,9 @@
       <c r="C48" s="0"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -1995,9 +2149,9 @@
       <c r="C49" s="0"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2014,9 +2168,9 @@
       <c r="C50" s="0"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2033,9 +2187,9 @@
       <c r="C51" s="0"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2052,9 +2206,9 @@
       <c r="C52" s="0"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2071,9 +2225,9 @@
       <c r="C53" s="0"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2088,27 +2242,27 @@
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
       <c r="C54" s="0"/>
-      <c r="V54" s="0"/>
-      <c r="W54" s="0"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0"/>
       <c r="B55" s="0"/>
       <c r="C55" s="0"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
+      <c r="V55" s="0"/>
+      <c r="W55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
@@ -2116,9 +2270,9 @@
       <c r="C56" s="0"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2135,9 +2289,9 @@
       <c r="C57" s="0"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2154,9 +2308,9 @@
       <c r="C58" s="0"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2173,9 +2327,9 @@
       <c r="C59" s="0"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2192,9 +2346,9 @@
       <c r="C60" s="0"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2211,9 +2365,9 @@
       <c r="C61" s="0"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2230,9 +2384,9 @@
       <c r="C62" s="0"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2249,9 +2403,9 @@
       <c r="C63" s="0"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2268,9 +2422,9 @@
       <c r="C64" s="0"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2287,9 +2441,9 @@
       <c r="C65" s="0"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2306,9 +2460,9 @@
       <c r="C66" s="0"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2325,9 +2479,9 @@
       <c r="C67" s="0"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2344,9 +2498,9 @@
       <c r="C68" s="0"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -2356,6 +2510,25 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0"/>
+      <c r="B69" s="0"/>
+      <c r="C69" s="0"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>